<commit_message>
Working on #15 to send business exception notification
</commit_message>
<xml_diff>
--- a/REFramework_Porreta/Data/Config.xlsx
+++ b/REFramework_Porreta/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/samuel_simao_uipath_com/Documents/Documents/UiPath/UiPath_REFramework_Porreta/REFramework_Porreta/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samuel.simao\OneDrive - UiPath\Documents\UiPath\UiPath_REFramework_Porreta\REFramework_Porreta\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71F12354-5082-496D-B4C1-CEC1E5523FDB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A7C0CB-02BF-4D89-87B6-76C84976D75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -169,13 +169,88 @@
   </si>
   <si>
     <t>MaxSystemExceptionsAtInitialization</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Data\BRE_Body.html</t>
+  </si>
+  <si>
+    <t>BRE_Notification_BodyHtmlFilePath</t>
+  </si>
+  <si>
+    <t>BRE in process</t>
+  </si>
+  <si>
+    <t>SE in Process</t>
+  </si>
+  <si>
+    <t>Exception in Initialization</t>
+  </si>
+  <si>
+    <t>Bot finished process</t>
+  </si>
+  <si>
+    <t>File path for the html file used as body in case of a business exception</t>
+  </si>
+  <si>
+    <t>BRE_Notification_Subject</t>
+  </si>
+  <si>
+    <t>Business exception happened</t>
+  </si>
+  <si>
+    <t>Subject used in case of a business exception</t>
+  </si>
+  <si>
+    <t>BRE_Notification_Recipients</t>
+  </si>
+  <si>
+    <t>; separated list of emails that will be notified in case of a business exception</t>
+  </si>
+  <si>
+    <t>samuelsimao47@gmail.com</t>
+  </si>
+  <si>
+    <t>BRE_Notification_CC</t>
+  </si>
+  <si>
+    <t>BRE_Notification_BCC</t>
+  </si>
+  <si>
+    <t>; separated list of emails that will be notified as CC in case of a business exception</t>
+  </si>
+  <si>
+    <t>; separated list of emails that will be notified as BCC in case of a business exception</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Boolean that toggles if a business exception in the process will trigger business exception</t>
+  </si>
+  <si>
+    <t>BRE_Notification_AttachmentsFolders</t>
+  </si>
+  <si>
+    <t>BRE_Notification_AttachmentsFiles</t>
+  </si>
+  <si>
+    <t>; separated list of folders whose files will be added as attachments in the business exception email</t>
+  </si>
+  <si>
+    <t>; separated list of files that will be added as attachments in the business exception email</t>
+  </si>
+  <si>
+    <t>BRE_Notification_Toggle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -199,6 +274,20 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -217,10 +306,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -230,8 +320,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -544,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -626,31 +719,120 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="20" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="13.5" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1617,10 +1799,15 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B17" r:id="rId1" xr:uid="{2D2582A4-1E76-4464-BBE0-C41AC0F932A0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1628,8 +1815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Finish sending BRE notification #15
</commit_message>
<xml_diff>
--- a/REFramework_Porreta/Data/Config.xlsx
+++ b/REFramework_Porreta/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samuel.simao\OneDrive - UiPath\Documents\UiPath\UiPath_REFramework_Porreta\REFramework_Porreta\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/samuel_simao_uipath_com/Documents/Documents/UiPath/UiPath_REFramework_Porreta/REFramework_Porreta/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A7C0CB-02BF-4D89-87B6-76C84976D75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{18A7C0CB-02BF-4D89-87B6-76C84976D75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCB9C363-EA4C-43BA-84A0-9E95A4CC33B6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Data\BRE_Body.html</t>
-  </si>
-  <si>
     <t>BRE_Notification_BodyHtmlFilePath</t>
   </si>
   <si>
@@ -225,32 +222,38 @@
     <t>; separated list of emails that will be notified as BCC in case of a business exception</t>
   </si>
   <si>
+    <t>Boolean that toggles if a business exception in the process will trigger business exception</t>
+  </si>
+  <si>
+    <t>; separated list of folders whose files will be added as attachments in the business exception email</t>
+  </si>
+  <si>
+    <t>; separated list of files that will be added as attachments in the business exception email</t>
+  </si>
+  <si>
+    <t>BRE_Notification_Toggle</t>
+  </si>
+  <si>
+    <t>notepad.exe</t>
+  </si>
+  <si>
+    <t>BRE_Notification_AttachmentFolders</t>
+  </si>
+  <si>
+    <t>BRE_Notification_AttachmentFiles</t>
+  </si>
+  <si>
+    <t>Data\HtmlTemplates\BRE_Body.html</t>
+  </si>
+  <si>
     <t>True</t>
-  </si>
-  <si>
-    <t>Boolean that toggles if a business exception in the process will trigger business exception</t>
-  </si>
-  <si>
-    <t>BRE_Notification_AttachmentsFolders</t>
-  </si>
-  <si>
-    <t>BRE_Notification_AttachmentsFiles</t>
-  </si>
-  <si>
-    <t>; separated list of folders whose files will be added as attachments in the business exception email</t>
-  </si>
-  <si>
-    <t>; separated list of files that will be added as attachments in the business exception email</t>
-  </si>
-  <si>
-    <t>BRE_Notification_Toggle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -281,13 +284,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -306,11 +302,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -321,10 +316,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -338,6 +331,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -637,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -718,111 +715,121 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="20" customHeight="1">
-      <c r="A8" s="5" t="s">
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="20" customHeight="1">
+      <c r="A9" s="5" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>53</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="13.5" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>67</v>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
+    <row r="14" spans="1:26" ht="13.5" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="C22" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1801,13 +1808,11 @@
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <hyperlinks>
-    <hyperlink ref="B17" r:id="rId1" xr:uid="{2D2582A4-1E76-4464-BBE0-C41AC0F932A0}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2988,7 +2993,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
BRE Body defined #15
</commit_message>
<xml_diff>
--- a/REFramework_Porreta/Data/Config.xlsx
+++ b/REFramework_Porreta/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/samuel_simao_uipath_com/Documents/Documents/UiPath/UiPath_REFramework_Porreta/REFramework_Porreta/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{18A7C0CB-02BF-4D89-87B6-76C84976D75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCB9C363-EA4C-43BA-84A0-9E95A4CC33B6}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{18A7C0CB-02BF-4D89-87B6-76C84976D75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AACC2F43-5723-436F-A871-C98BE20CF334}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -637,7 +637,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Trying to add a separate style.css for email body, NOT WORKED #15, #18, #6
</commit_message>
<xml_diff>
--- a/REFramework_Porreta/Data/Config.xlsx
+++ b/REFramework_Porreta/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/samuel_simao_uipath_com/Documents/Documents/UiPath/UiPath_REFramework_Porreta/REFramework_Porreta/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{18A7C0CB-02BF-4D89-87B6-76C84976D75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AACC2F43-5723-436F-A871-C98BE20CF334}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{18A7C0CB-02BF-4D89-87B6-76C84976D75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67BA1811-F974-4D2B-AE50-B496F26604E0}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
   <si>
     <t>Name</t>
   </si>
@@ -247,6 +247,60 @@
   </si>
   <si>
     <t>True</t>
+  </si>
+  <si>
+    <t>SE_Notification_Toggle</t>
+  </si>
+  <si>
+    <t>SE_Notification_BodyHtmlFilePath</t>
+  </si>
+  <si>
+    <t>SE_Notification_Subject</t>
+  </si>
+  <si>
+    <t>SE_Notification_Recipients</t>
+  </si>
+  <si>
+    <t>SE_Notification_CC</t>
+  </si>
+  <si>
+    <t>SE_Notification_BCC</t>
+  </si>
+  <si>
+    <t>SE_Notification_AttachmentFolders</t>
+  </si>
+  <si>
+    <t>SE_Notification_AttachmentFiles</t>
+  </si>
+  <si>
+    <t>Data\HtmlTemplates\SE_Body.html</t>
+  </si>
+  <si>
+    <t>System exception happened</t>
+  </si>
+  <si>
+    <t>Boolean that toggles if a system exception in the process will trigger system exception</t>
+  </si>
+  <si>
+    <t>File path for the html file used as body in case of a system exception</t>
+  </si>
+  <si>
+    <t>Subject used in case of a susiness exception</t>
+  </si>
+  <si>
+    <t>; separated list of emails that will be notified in case of a susiness exception</t>
+  </si>
+  <si>
+    <t>; separated list of emails that will be notified as CC in case of a susiness exception</t>
+  </si>
+  <si>
+    <t>; separated list of emails that will be notified as BCC in case of a susiness exception</t>
+  </si>
+  <si>
+    <t>; separated list of folders whose files will be added as attachments in the susiness exception email</t>
+  </si>
+  <si>
+    <t>; separated list of files that will be added as attachments in the susiness exception email</t>
   </si>
 </sst>
 </file>
@@ -636,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -831,14 +885,82 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
@@ -1820,8 +1942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Config refactored to Json in initialization #16
</commit_message>
<xml_diff>
--- a/REFramework_Porreta/Data/Config.xlsx
+++ b/REFramework_Porreta/Data/Config.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{18A7C0CB-02BF-4D89-87B6-76C84976D75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67BA1811-F974-4D2B-AE50-B496F26604E0}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="100" yWindow="100" windowWidth="19190" windowHeight="10070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -690,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1942,8 +1942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3115,7 +3115,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>